<commit_message>
1) Final slides for ECE803 presentation 2) More work (final?) on the energy analysis spreadsheet
</commit_message>
<xml_diff>
--- a/Documentation/Results/IODVS/EnergyAnalysis.xlsx
+++ b/Documentation/Results/IODVS/EnergyAnalysis.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12960" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="6" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="5" r:id="rId6"/>
+    <sheet name="EEPROM" sheetId="1" r:id="rId1"/>
+    <sheet name="SerialFlash" sheetId="2" r:id="rId2"/>
+    <sheet name="Sandisk" sheetId="3" r:id="rId3"/>
+    <sheet name="Lexar" sheetId="9" r:id="rId4"/>
+    <sheet name="SwissBit" sheetId="10" r:id="rId5"/>
+    <sheet name="Kingston" sheetId="11" r:id="rId6"/>
+    <sheet name="HIH6130" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="33">
   <si>
     <t>Idle</t>
   </si>
@@ -109,6 +110,21 @@
   <si>
     <t>SwissBit SDCard Read/Modify/Write Energy Consumption</t>
   </si>
+  <si>
+    <t>Write Complete / Verify</t>
+  </si>
+  <si>
+    <t>%Change</t>
+  </si>
+  <si>
+    <t>Static (uJ)</t>
+  </si>
+  <si>
+    <t>IODVS (uJ)</t>
+  </si>
+  <si>
+    <t>Energy Usage</t>
+  </si>
 </sst>
 </file>
 
@@ -150,20 +166,41 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -182,13 +219,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -539,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1328,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
@@ -4510,1437 +4557,962 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="F14:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
-    <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="E3" s="6"/>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>114.68728810717801</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>102.608352567336</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>B4</f>
+        <v>114.68728810717801</v>
+      </c>
+      <c r="H4">
+        <f>D4</f>
+        <v>102.608352567336</v>
+      </c>
+      <c r="I4">
+        <f>100*((H4/G4)-1)</f>
+        <v>-10.532061346287968</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>20.022635268297901</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>18.916046009165498</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G6" si="0">B5</f>
+        <v>20.022635268297901</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H6" si="1">D5</f>
+        <v>18.916046009165498</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I8" si="2">100*((H5/G5)-1)</f>
+        <v>-5.526691388543048</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>10899.2687815564</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>6553.0588152423497</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>10899.2687815564</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>6553.0588152423497</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>-39.876160992273633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>66.878091309646706</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>66.143239129507407</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7">
+        <f>B7+B8+B9</f>
+        <v>75.524086204635751</v>
+      </c>
+      <c r="H7">
+        <f>SUM(D7:D9)</f>
+        <v>86.331451885661437</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>14.30982647276613</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8">
+        <v>1.4942931745308401</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>3.0594014915445298</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <f>B10</f>
+        <v>11109.5027911365</v>
+      </c>
+      <c r="H8">
+        <f>D10</f>
+        <v>6760.9146657045103</v>
+      </c>
+      <c r="I8">
+        <f>100*((H8/G8)-1)</f>
+        <v>-39.142959025145807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9">
+        <v>7.1517017204581999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>17.128811264609499</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10">
+        <v>11109.5027911365</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>6760.9146657045103</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
-      <c r="B4">
-        <v>110.350725821449</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>99.369449782575103</v>
-      </c>
-      <c r="G4">
-        <v>46.6386749708713</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>25.807938587131201</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4">
-        <v>44.664082752672897</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="B5">
-        <v>19.931364264154599</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5">
-        <v>18.858739386730601</v>
-      </c>
-      <c r="G5">
-        <v>42.879939502175397</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5">
-        <v>50.268223187085603</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5">
-        <v>-17.2301634999633</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="B6">
-        <v>10893.329243816101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6">
-        <v>6606.3530380623997</v>
-      </c>
-      <c r="G6">
-        <v>24.921969175683699</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6">
-        <v>24.739382147979601</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6">
-        <v>0.73263483481984504</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="B7">
-        <v>13.851745244061</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>1.20817938956209</v>
-      </c>
-      <c r="G7">
-        <v>12784.6945390824</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7">
-        <v>7981.2346714369296</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7">
-        <v>37.571956474685003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="B8">
-        <v>8.4117563752354592</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8">
-        <v>7.6025835520290697</v>
-      </c>
-      <c r="G8">
-        <v>54.409273233156298</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8">
-        <v>59.1773098317937</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8">
-        <v>-8.7632793369713404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="B9">
-        <v>11045.874835520999</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>6733.3919901732997</v>
-      </c>
-      <c r="G9">
-        <v>77.515472110521699</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9">
-        <v>79.222536852934496</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9">
-        <v>-2.2022245313539899</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="G10">
-        <v>75.027053719933207</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10">
-        <v>84.174570641433704</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10">
-        <v>-12.1922912708889</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="G11">
-        <v>120.932704447253</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11">
-        <v>114.91826517502</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11">
-        <v>4.9733769700455301</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12">
-        <v>29.811772781054302</v>
-      </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12">
-        <v>27.3913585795293</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12">
-        <v>8.1189878216943292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="G13">
-        <v>13256.8313990231</v>
-      </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13">
-        <v>8446.9342564398394</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13">
-        <v>36.282404126657902</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="B14">
-        <v>151.55297198862499</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>133.58174530442199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+    <row r="14" spans="1:9">
+      <c r="E14" s="6"/>
+      <c r="F14" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="B15">
-        <v>26.541508618798598</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
+        <v>157.07123335679501</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>26.2911987992462</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>138.952913872838</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
+        <f>B15</f>
+        <v>157.07123335679501</v>
+      </c>
+      <c r="H15" s="10">
+        <f>D15</f>
+        <v>138.952913872838</v>
+      </c>
+      <c r="I15" s="12">
+        <f>((H15/G15)-1)</f>
+        <v>-0.11535097227383684</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16">
-        <v>13995.1431116761</v>
+        <v>26.4798983715189</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>10126.3909037673</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="J16" t="s">
-        <v>14</v>
-      </c>
-      <c r="K16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>26.234707562508699</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" ref="G16:G17" si="3">B16</f>
+        <v>26.4798983715189</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" ref="H16:H17" si="4">D16</f>
+        <v>26.234707562508699</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" ref="I16:I19" si="5">((H16/G16)-1)</f>
+        <v>-9.2595071767315185E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17">
-        <v>26.204655194633499</v>
+        <v>14021.9688782512</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17">
-        <v>5.1981580368854496</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>10126.954813652201</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="3"/>
+        <v>14021.9688782512</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="4"/>
+        <v>10126.954813652201</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="5"/>
+        <v>-0.27777939734557311</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18">
-        <v>16.4450616879992</v>
+        <v>87.264044543905499</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18">
-        <v>12.343287579334</v>
-      </c>
-      <c r="G18">
-        <v>65.786322066470802</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>43.0701547567378</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>100</v>
-      </c>
-      <c r="M18">
-        <v>34.530228467219203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>87.822739176491694</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="10">
+        <f>B18+B19</f>
+        <v>89.85558882025876</v>
+      </c>
+      <c r="H18" s="10">
+        <f>SUM(D18:D19)</f>
+        <v>91.87934878285337</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="5"/>
+        <v>2.2522360480468295E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19">
-        <v>14215.887309166201</v>
+        <v>2.5915442763532601</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19">
-        <v>10303.805293487199</v>
-      </c>
-      <c r="G19">
-        <v>57.338976933382597</v>
-      </c>
-      <c r="H19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19">
-        <v>58.515046208200097</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19">
-        <v>-2.0510817208754002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="G20">
-        <v>32.9692001953212</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20">
-        <v>32.866878428271598</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20">
-        <v>0.31035562416874601</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="G21">
-        <v>16283.234023472</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21">
-        <v>12243.3434013632</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21">
-        <v>24.810124427895701</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22">
-        <v>69.673429190015398</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22">
-        <v>68.825949807124601</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22">
-        <v>1.2163595114279699</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="G23">
-        <v>100.711594530762</v>
-      </c>
-      <c r="H23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23">
-        <v>102.030812477583</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23">
-        <v>-1.3098967928840901</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-      <c r="D24">
-        <v>9.9512494885098004</v>
-      </c>
-      <c r="G24">
-        <v>105.364098035452</v>
-      </c>
-      <c r="H24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24">
-        <v>115.824416589325</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24">
-        <v>-9.9277825643739899</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25">
-        <v>5.3815928664400703</v>
-      </c>
-      <c r="G25">
-        <v>168.26962968361801</v>
-      </c>
-      <c r="H25" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25">
-        <v>161.36026437985299</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>24</v>
-      </c>
-      <c r="M25">
-        <v>4.1061273604489097</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26">
-        <v>39.354141509927203</v>
-      </c>
-      <c r="G26">
-        <v>40.894462665462697</v>
-      </c>
-      <c r="H26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26">
-        <v>37.292229295589102</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26">
-        <v>8.8086091247652494</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27">
-        <v>91.277782198022294</v>
-      </c>
-      <c r="G27">
-        <v>16924.241736772499</v>
-      </c>
-      <c r="H27" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27">
-        <v>12863.129153305899</v>
-      </c>
-      <c r="K27">
-        <v>0</v>
-      </c>
-      <c r="L27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27">
-        <v>23.995831817048501</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28">
-        <v>9.6195465858786093</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29">
-        <v>39.041568998045499</v>
-      </c>
+        <v>4.0566096063616799</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="11">
+        <f>SUM(G15:G18)</f>
+        <v>14295.375598799774</v>
+      </c>
+      <c r="H19" s="11">
+        <f>SUM(H15:H18)</f>
+        <v>10384.021783870401</v>
+      </c>
+      <c r="I19" s="13">
+        <f t="shared" si="5"/>
+        <v>-0.27360972699855235</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20">
+        <v>32.723085833136999</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>46.112152737500303</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21">
+        <v>14328.0986846329</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>10430.133936607899</v>
+      </c>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
-    <col min="7" max="7" width="12.25" customWidth="1"/>
+    <col min="6" max="6" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="10.25" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="9.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="E3" s="6"/>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="B4">
-        <v>88.587878026745898</v>
+        <v>90.743977909370102</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>75.182412874053497</v>
+        <v>76.111714750552693</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" t="s">
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>43.237237021504399</v>
+        <f>B4</f>
+        <v>90.743977909370102</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <f>D4</f>
+        <v>76.111714750552693</v>
       </c>
       <c r="I4">
-        <v>25.051940815057399</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4">
-        <v>42.059339262132902</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <f>100*((H4/G4)-1)</f>
+        <v>-16.124775986161065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5">
-        <v>26.520355347915601</v>
+        <v>25.9951021218695</v>
       </c>
       <c r="C5" t="s">
         <v>24</v>
       </c>
       <c r="D5">
-        <v>25.696322511561998</v>
+        <v>25.385346904715099</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
       <c r="G5">
-        <v>68.740833337786995</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
+        <f t="shared" ref="G5:G6" si="0">B5</f>
+        <v>25.9951021218695</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H6" si="1">D5</f>
+        <v>25.385346904715099</v>
       </c>
       <c r="I5">
-        <v>75.904394639599403</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5">
-        <v>-10.421115011235299</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <f t="shared" ref="I5:I7" si="2">100*((H5/G5)-1)</f>
+        <v>-2.3456542478493159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="B6">
-        <v>12914.708076434201</v>
+        <v>13007.9604444051</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6">
-        <v>8116.7514064812303</v>
+        <v>8182.6686607891397</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s">
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>18.392774725867501</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>13007.9604444051</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>8182.6686607891397</v>
       </c>
       <c r="I6">
-        <v>17.330958981378</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6">
-        <v>5.7730046733853904</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <f t="shared" si="2"/>
+        <v>-37.094914335255261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7">
-        <v>217.031065933788</v>
+        <v>2.7619763446400101</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7">
-        <v>218.20301261161501</v>
+        <v>1.8136451676974199</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" t="s">
+        <v>28</v>
       </c>
       <c r="G7">
-        <v>10506.5590691739</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
+        <f>B7+B8</f>
+        <v>10.40743648439901</v>
+      </c>
+      <c r="H7">
+        <f>D7+D8</f>
+        <v>24.22004941565082</v>
       </c>
       <c r="I7">
-        <v>6305.9941168069599</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7">
-        <v>39.980405808513801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <f t="shared" si="2"/>
+        <v>132.71868583543355</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="B8">
-        <v>6.60831293019789</v>
+        <v>7.6454601397589999</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
       </c>
       <c r="D8">
-        <v>6.3047332517130901</v>
+        <v>22.4064042479534</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" t="s">
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>387.91459798194597</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
+        <f>B9</f>
+        <v>13135.106960920701</v>
+      </c>
+      <c r="H8">
+        <f>D9</f>
+        <v>8308.3857718600593</v>
       </c>
       <c r="I8">
-        <v>301.37669421923698</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8">
-        <v>22.308493728492301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <f>100*((H8/G8)-1)</f>
+        <v>-36.746721617273479</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="B9">
-        <v>13253.455688672901</v>
+        <v>13135.106960920701</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9">
-        <v>8442.1378877301795</v>
-      </c>
-      <c r="G9">
-        <v>8.9990351114659806</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9">
-        <v>0.462568345650822</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9">
-        <v>94.859800635054199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="G10">
-        <v>5.0194558271609298</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10">
-        <v>0.77186132351058001</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10">
-        <v>84.622609500138694</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="G11">
-        <v>8.3711273779931901</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11">
-        <v>7.58500814896479</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11">
-        <v>9.3908406064280303</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
+        <v>8308.3857718600593</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12">
-        <v>3.57809750508962E-3</v>
-      </c>
-      <c r="K12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13">
-        <v>3.5780975050895502E-3</v>
-      </c>
-      <c r="K13" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13" s="6"/>
+      <c r="F13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="B14">
-        <v>120.75056862611299</v>
+        <v>124.089837064118</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>99.284527603111599</v>
-      </c>
-      <c r="G14" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14">
-        <v>6734.4846994753698</v>
-      </c>
-      <c r="K14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
+        <v>102.41393567405299</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <f>B14</f>
+        <v>124.089837064118</v>
+      </c>
+      <c r="H14" s="10">
+        <f>D14</f>
+        <v>102.41393567405299</v>
+      </c>
+      <c r="I14" s="12">
+        <f>((H14/G14)-1)</f>
+        <v>-0.17467910267997966</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="B15">
-        <v>35.174945849624102</v>
+        <v>34.5163581887766</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15">
-        <v>34.929094238832903</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+        <v>34.420818587428499</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" ref="G15:G16" si="3">B15</f>
+        <v>34.5163581887766</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" ref="H15:H16" si="4">D15</f>
+        <v>34.420818587428499</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" ref="I15:I18" si="5">((H15/G15)-1)</f>
+        <v>-2.767951381938305E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16">
-        <v>16451.573980179401</v>
+        <v>16608.429094285199</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
       </c>
       <c r="D16">
-        <v>12412.1363326714</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+        <v>12558.834192018199</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="3"/>
+        <v>16608.429094285199</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="4"/>
+        <v>12558.834192018199</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" si="5"/>
+        <v>-0.24382769010107197</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17">
-        <v>303.236113574461</v>
+        <v>3.7458423968538499</v>
       </c>
       <c r="C17" t="s">
         <v>24</v>
       </c>
       <c r="D17">
-        <v>303.90985292019002</v>
-      </c>
-      <c r="F17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+        <v>2.3544569083529199</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="10">
+        <f>B17+B18</f>
+        <v>39.446955199612653</v>
+      </c>
+      <c r="H17" s="10">
+        <f>D17+D18</f>
+        <v>56.872557622500224</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="5"/>
+        <v>0.44174771752874564</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18">
-        <v>8.4024478056779692</v>
+        <v>35.7011128027588</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18">
-        <v>7.9496228689161601</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>54.518100714147302</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="11">
+        <f>B19</f>
+        <v>16806.482244737701</v>
+      </c>
+      <c r="H18" s="11">
+        <f>D19</f>
+        <v>12752.541503902199</v>
+      </c>
+      <c r="I18" s="13">
+        <f t="shared" si="5"/>
+        <v>-0.24121292497749414</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19">
-        <v>16919.138056035201</v>
+        <v>16806.482244737701</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19">
-        <v>12858.209430302501</v>
-      </c>
-      <c r="G19">
-        <v>60.7500285855238</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>41.638620292408604</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>100</v>
-      </c>
-      <c r="M19">
-        <v>31.459093498548999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="G20">
-        <v>92.937661371401006</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20">
-        <v>94.063839918777802</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20">
-        <v>-1.21175692475883</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="G21">
-        <v>24.553825325586999</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21">
-        <v>24.2883959345953</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21">
-        <v>1.08101034145236</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22">
-        <v>13482.7731943338</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22">
-        <v>9724.3055391800408</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22">
-        <v>27.876072681644601</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="G23">
-        <v>513.83482066501006</v>
-      </c>
-      <c r="H23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23">
-        <v>403.41143978649598</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23">
-        <v>21.4900540869541</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-      <c r="D24">
-        <v>15.132392209061701</v>
-      </c>
-      <c r="G24">
-        <v>15.441339627235701</v>
-      </c>
-      <c r="H24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24">
-        <v>2.06844627751369</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>24</v>
-      </c>
-      <c r="M24">
-        <v>86.604489458509605</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25">
-        <v>3.10717117302254</v>
-      </c>
-      <c r="G25">
-        <v>11.130242021500001</v>
-      </c>
-      <c r="H25" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25">
-        <v>3.2408269710428699</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>24</v>
-      </c>
-      <c r="M25">
-        <v>70.882690917388302</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26">
-        <v>37.151104318865201</v>
-      </c>
-      <c r="G26">
-        <v>16.314835149016499</v>
-      </c>
-      <c r="H26" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26">
-        <v>12.273532609293801</v>
-      </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
-        <v>24</v>
-      </c>
-      <c r="M26">
-        <v>24.770722491587001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27">
-        <v>-0.539990287927128</v>
-      </c>
-      <c r="G27" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27">
-        <v>3.7651775832948401E-3</v>
-      </c>
-      <c r="K27" t="s">
-        <v>24</v>
-      </c>
-      <c r="L27" t="s">
-        <v>24</v>
-      </c>
-      <c r="M27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28">
-        <v>4.5939059135280802</v>
-      </c>
-      <c r="G28" t="s">
-        <v>24</v>
-      </c>
-      <c r="H28" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28">
-        <v>3.7651775832947699E-3</v>
-      </c>
-      <c r="K28" t="s">
-        <v>24</v>
-      </c>
-      <c r="L28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29">
-        <v>36.3023645603215</v>
-      </c>
-      <c r="G29" t="s">
-        <v>24</v>
-      </c>
-      <c r="H29" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29">
-        <v>10305.298171325299</v>
-      </c>
-      <c r="K29" t="s">
-        <v>24</v>
-      </c>
-      <c r="L29" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="A32" t="s">
-        <v>14</v>
-      </c>
-      <c r="B32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34">
-        <v>100</v>
-      </c>
-      <c r="D34">
-        <v>17.777175931541599</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35">
-        <v>0.69893955726961798</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36">
-        <v>24.5535026154615</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37">
-        <v>-0.22218308294035299</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4">
-      <c r="B38">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38">
-        <v>5.3892026137408298</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4">
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39">
-        <v>24.0019829159334</v>
-      </c>
+        <v>12752.541503902199</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="G20" sqref="G20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="13.75" customWidth="1"/>
+    <col min="7" max="7" width="10.125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="E3" s="6"/>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="B4">
         <v>48.012705717838301</v>
       </c>
@@ -5950,26 +5522,24 @@
       <c r="D4">
         <v>26.9989596466941</v>
       </c>
+      <c r="E4" s="6"/>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
       <c r="G4">
+        <f>B4</f>
         <v>48.012705717838301</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <f>D4</f>
+        <v>26.9989596466941</v>
       </c>
       <c r="I4">
-        <v>26.9989596466941</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>100</v>
-      </c>
-      <c r="M4">
-        <v>43.767052401999699</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <f>100*((H4/G4)-1)</f>
+        <v>-43.767052401999706</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="B5">
         <v>11.173622664239</v>
       </c>
@@ -5979,113 +5549,105 @@
       <c r="D5">
         <v>17.250556149698301</v>
       </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
       <c r="G5">
-        <v>11.173622664239</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
+        <f>B5+B6</f>
+        <v>19.80276004914279</v>
+      </c>
+      <c r="H5">
+        <f>D5+D6</f>
+        <v>25.935972584517003</v>
       </c>
       <c r="I5">
-        <v>17.250556149698301</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5">
-        <v>-54.386421199889199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <f t="shared" ref="I5:I7" si="0">100*((H5/G5)-1)</f>
+        <v>30.971503568966916</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="B6">
-        <v>8.2497234164995294</v>
+        <v>8.6291373849037907</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6">
-        <v>8.3139951371078595</v>
+        <v>8.6854164348187002</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s">
+        <v>18</v>
       </c>
       <c r="G6">
-        <v>8.2497234164995294</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
+        <f>B7</f>
+        <v>2900.5765198664499</v>
+      </c>
+      <c r="H6">
+        <f>D7</f>
+        <v>1839.35038723757</v>
       </c>
       <c r="I6">
-        <v>8.3139951371078595</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6">
-        <v>-0.77907727766710599</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <f t="shared" si="0"/>
+        <v>-36.586731132945303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7">
-        <v>2901.4565027231301</v>
+        <v>2900.5765198664499</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7">
-        <v>1844.2761896305601</v>
+        <v>1839.35038723757</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" t="s">
+        <v>28</v>
       </c>
       <c r="G7">
-        <v>2901.4565027231301</v>
-      </c>
-      <c r="H7" t="s">
-        <v>24</v>
+        <f>B8+B9+B10</f>
+        <v>39.991418759278005</v>
+      </c>
+      <c r="H7">
+        <f>D8+D9+D10</f>
+        <v>44.864493961154999</v>
       </c>
       <c r="I7">
-        <v>1844.2761896305601</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7">
-        <v>36.436193756492898</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <f t="shared" si="0"/>
+        <v>12.18530212996367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="B8">
-        <v>11.2475550347444</v>
+        <v>11.8129270487665</v>
       </c>
       <c r="C8" t="s">
         <v>24</v>
       </c>
       <c r="D8">
-        <v>13.4498160234113</v>
+        <v>16.6939492652021</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" t="s">
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>11.2475550347444</v>
-      </c>
-      <c r="H8" t="s">
-        <v>24</v>
+        <f>B11</f>
+        <v>3008.38340439271</v>
+      </c>
+      <c r="H8">
+        <f>D11</f>
+        <v>1937.14981342993</v>
       </c>
       <c r="I8">
-        <v>13.4498160234113</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8">
-        <v>-19.579908538913099</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
+        <f>100*((H8/G8)-1)</f>
+        <v>-35.608280161318916</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="B9">
         <v>15.917350085189501</v>
       </c>
@@ -6095,26 +5657,9 @@
       <c r="D9">
         <v>13.704121751261599</v>
       </c>
-      <c r="G9">
-        <v>15.917350085189501</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9">
-        <v>13.704121751261599</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9">
-        <v>13.9045024585297</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="B10">
         <v>12.261141625322001</v>
       </c>
@@ -6124,75 +5669,51 @@
       <c r="D10">
         <v>14.466422944691301</v>
       </c>
-      <c r="G10">
-        <v>12.261141625322001</v>
-      </c>
-      <c r="H10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10">
-        <v>14.466422944691301</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M10">
-        <v>-17.9859379065886</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="B11">
-        <v>3008.3186012669598</v>
+        <v>3008.38340439271</v>
       </c>
       <c r="C11" t="s">
         <v>24</v>
       </c>
       <c r="D11">
-        <v>1938.4600612834299</v>
-      </c>
-      <c r="G11">
-        <v>3008.3186012669598</v>
-      </c>
-      <c r="H11" t="s">
-        <v>24</v>
-      </c>
-      <c r="I11">
-        <v>1938.4600612834299</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11">
-        <v>35.563338920716603</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
+        <v>1937.14981342993</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="J14" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="E15" s="6"/>
+      <c r="F15" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16">
         <v>66.248256436440101</v>
       </c>
@@ -6202,26 +5723,24 @@
       <c r="D16">
         <v>43.5282630245161</v>
       </c>
-      <c r="G16">
+      <c r="E16" s="6"/>
+      <c r="F16" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <f>B16</f>
         <v>66.248256436440101</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
+      <c r="H16" s="10">
+        <f>D16</f>
         <v>43.5282630245161</v>
       </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>100</v>
-      </c>
-      <c r="M16">
-        <v>34.295232258258899</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="I16" s="12">
+        <f>((H16/G16)-1)</f>
+        <v>-0.34295232258258779</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
       <c r="B17">
         <v>14.3050863086983</v>
       </c>
@@ -6231,113 +5750,105 @@
       <c r="D17">
         <v>14.993531787857901</v>
       </c>
-      <c r="G17">
-        <v>14.3050863086983</v>
-      </c>
-      <c r="H17" t="s">
-        <v>24</v>
-      </c>
-      <c r="I17">
-        <v>14.993531787857901</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17">
-        <v>-4.8125922787407802</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="E17" s="6"/>
+      <c r="F17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="10">
+        <f>B17+B18</f>
+        <v>25.007347276605302</v>
+      </c>
+      <c r="H17" s="10">
+        <f>D17+D18</f>
+        <v>25.719039196703498</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" ref="I17:I20" si="1">((H17/G17)-1)</f>
+        <v>2.8459312866182973E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
       <c r="B18">
-        <v>10.2295685014799</v>
+        <v>10.702260967907</v>
       </c>
       <c r="C18" t="s">
         <v>24</v>
       </c>
       <c r="D18">
-        <v>10.2436559415608</v>
-      </c>
-      <c r="G18">
-        <v>10.2295685014799</v>
-      </c>
-      <c r="H18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I18">
-        <v>10.2436559415608</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18" t="s">
-        <v>24</v>
-      </c>
-      <c r="M18">
-        <v>-0.13771294535862599</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+        <v>10.725507408845599</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="10">
+        <f>B19</f>
+        <v>3726.2018823028902</v>
+      </c>
+      <c r="H18" s="10">
+        <f>D19</f>
+        <v>2839.7783376861698</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.23788929655869517</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
       <c r="B19">
-        <v>3727.3709297639898</v>
+        <v>3726.2018823028902</v>
       </c>
       <c r="C19" t="s">
         <v>24</v>
       </c>
       <c r="D19">
-        <v>2841.5666053371501</v>
-      </c>
-      <c r="G19">
-        <v>3727.3709297639898</v>
-      </c>
-      <c r="H19" t="s">
-        <v>24</v>
-      </c>
-      <c r="I19">
-        <v>2841.5666053371501</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19" t="s">
-        <v>24</v>
-      </c>
-      <c r="M19">
-        <v>23.764855741978199</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
+        <v>2839.7783376861698</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="10">
+        <f>B20+B21</f>
+        <v>36.307266812242204</v>
+      </c>
+      <c r="H19" s="10">
+        <f>D20+D21</f>
+        <v>31.680621328512199</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.12743028847795224</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
       <c r="B20">
-        <v>14.7079223907488</v>
+        <v>15.410425380621501</v>
       </c>
       <c r="C20" t="s">
         <v>24</v>
       </c>
       <c r="D20">
-        <v>13.4697342603379</v>
-      </c>
-      <c r="G20">
-        <v>14.7079223907488</v>
-      </c>
-      <c r="H20" t="s">
-        <v>24</v>
-      </c>
-      <c r="I20">
-        <v>13.4697342603379</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20" t="s">
-        <v>24</v>
-      </c>
-      <c r="M20">
-        <v>8.4185114492425903</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+        <v>14.456043441368699</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="11">
+        <f>SUM(G16:G19)</f>
+        <v>3853.7647528281777</v>
+      </c>
+      <c r="H20" s="11">
+        <f>SUM(H16:H19)</f>
+        <v>2940.7062612359018</v>
+      </c>
+      <c r="I20" s="13">
+        <f t="shared" si="1"/>
+        <v>-0.23692636944748791</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
       <c r="B21">
         <v>20.8968414316207</v>
       </c>
@@ -6347,26 +5858,9 @@
       <c r="D21">
         <v>17.2245778871435</v>
       </c>
-      <c r="G21">
-        <v>20.8968414316207</v>
-      </c>
-      <c r="H21" t="s">
-        <v>24</v>
-      </c>
-      <c r="I21">
-        <v>17.2245778871435</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
-      <c r="L21" t="s">
-        <v>24</v>
-      </c>
-      <c r="M21">
-        <v>17.5732947799487</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:9">
       <c r="B22">
         <v>38.272207601993998</v>
       </c>
@@ -6376,260 +5870,596 @@
       <c r="D22">
         <v>40.911188090904197</v>
       </c>
-      <c r="G22">
-        <v>38.272207601993998</v>
-      </c>
-      <c r="H22" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22">
-        <v>40.911188090904197</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22">
-        <v>-6.8952920520130503</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:9">
       <c r="B23">
-        <v>3892.0308124349699</v>
+        <v>3892.03696043017</v>
       </c>
       <c r="C23" t="s">
         <v>24</v>
       </c>
       <c r="D23">
-        <v>2981.9375563294702</v>
-      </c>
-      <c r="G23">
-        <v>3892.0308124349699</v>
-      </c>
-      <c r="H23" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23">
-        <v>2981.9375563294702</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23">
-        <v>23.383505937254501</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>100</v>
-      </c>
-      <c r="D28">
-        <v>43.767052401999699</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29">
-        <v>-54.386421199889199</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13">
-      <c r="B30">
-        <v>0</v>
-      </c>
-      <c r="C30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30">
-        <v>-0.77907727766710599</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13">
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31">
-        <v>36.436193756492898</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13">
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32">
-        <v>-19.579908538913099</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33">
-        <v>13.9045024585297</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="B34">
-        <v>0</v>
-      </c>
-      <c r="C34" t="s">
-        <v>24</v>
-      </c>
-      <c r="D34">
-        <v>-17.9859379065886</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="B35">
-        <v>0</v>
-      </c>
-      <c r="C35" t="s">
-        <v>24</v>
-      </c>
-      <c r="D35">
-        <v>35.563338920716603</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>14</v>
-      </c>
-      <c r="B38" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="B40">
-        <v>0</v>
-      </c>
-      <c r="C40">
-        <v>100</v>
-      </c>
-      <c r="D40">
-        <v>34.295232258258899</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="B41">
-        <v>0</v>
-      </c>
-      <c r="C41" t="s">
-        <v>24</v>
-      </c>
-      <c r="D41">
-        <v>-4.8125922787407802</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="B42">
-        <v>0</v>
-      </c>
-      <c r="C42" t="s">
-        <v>24</v>
-      </c>
-      <c r="D42">
-        <v>-0.13771294535862599</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43">
-        <v>23.764855741978199</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44">
-        <v>8.4185114492425903</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="B45">
-        <v>0</v>
-      </c>
-      <c r="C45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D45">
-        <v>17.5732947799487</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46">
-        <v>-6.8952920520130503</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="B47">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47">
-        <v>23.383505937254501</v>
-      </c>
+        <v>2981.6174493268099</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I43"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="6" max="6" width="13.25" customWidth="1"/>
+    <col min="7" max="7" width="8.625" customWidth="1"/>
+    <col min="8" max="8" width="10.625" customWidth="1"/>
+    <col min="9" max="9" width="8.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="E3" s="6"/>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="B4">
+        <v>17.394062079219999</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>10.0916045808279</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>B4</f>
+        <v>17.394062079219999</v>
+      </c>
+      <c r="H4">
+        <f>D4</f>
+        <v>10.0916045808279</v>
+      </c>
+      <c r="I4">
+        <f>100*((H4/G4)-1)</f>
+        <v>-41.982473473611769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="B5">
+        <v>40.562918370685701</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>47.5443754198295</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5">
+        <f>B5+B6</f>
+        <v>68.843027345025206</v>
+      </c>
+      <c r="H5">
+        <f>D5+D6</f>
+        <v>75.838541365579701</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I7" si="0">100*((H5/G5)-1)</f>
+        <v>10.161543282364116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="B6">
+        <v>28.280108974339502</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>28.294165945750201</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6">
+        <f>B7</f>
+        <v>94.3709368992847</v>
+      </c>
+      <c r="H6">
+        <f>D7</f>
+        <v>64.556424797333307</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>-31.592896162268978</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="B7">
+        <v>94.3709368992847</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>64.556424797333307</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7">
+        <f>B8+B9+B10</f>
+        <v>41.287511566016434</v>
+      </c>
+      <c r="H7">
+        <f>D8+D9+D10</f>
+        <v>43.998733349541247</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>6.5666873121905667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="B8">
+        <v>40.287689038378701</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>43.003088847005998</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <f>SUM(G4:G7)</f>
+        <v>221.89553788954632</v>
+      </c>
+      <c r="H8">
+        <f>SUM(H4:H7)</f>
+        <v>194.48530409328217</v>
+      </c>
+      <c r="I8">
+        <f>100*((H8/G8)-1)</f>
+        <v>-12.352764754516265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="B9">
+        <v>0.44693550966704898</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>0.44034295887225799</v>
+      </c>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="B10">
+        <v>0.55288701797068396</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>0.555301543662992</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11">
+        <v>7.6986981498102001</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>22.086896087865401</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="B12">
+        <v>229.59423603935701</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12">
+        <v>216.57220018114799</v>
+      </c>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="B16">
+        <v>24.626114138781201</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>16.893505156614101</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17">
+        <v>53.209857606824499</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>54.910946065489298</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <f>B16</f>
+        <v>24.626114138781201</v>
+      </c>
+      <c r="H17" s="10">
+        <f>D16</f>
+        <v>16.893505156614101</v>
+      </c>
+      <c r="I17" s="12">
+        <f>((H17/G17)-1)</f>
+        <v>-0.3140003712558852</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18">
+        <v>36.529551416184297</v>
+      </c>
+      <c r="C18" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18">
+        <v>36.536753584013397</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="10">
+        <f>B17+B18</f>
+        <v>89.73940902300879</v>
+      </c>
+      <c r="H18" s="10">
+        <f>D17+D18</f>
+        <v>91.447699649502695</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" ref="I18:I21" si="1">((H18/G18)-1)</f>
+        <v>1.9036125210674326E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19">
+        <v>122.44205034861901</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>97.386326573772905</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="10">
+        <f>B19</f>
+        <v>122.44205034861901</v>
+      </c>
+      <c r="H19" s="10">
+        <f>D19</f>
+        <v>97.386326573772905</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.2046333241195083</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20">
+        <v>52.7138153750643</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>56.226042377950797</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="10">
+        <f>B20+B21+B22</f>
+        <v>54.001622609508544</v>
+      </c>
+      <c r="H20" s="10">
+        <f>D20+D21+D22</f>
+        <v>57.530166176385315</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="1"/>
+        <v>6.5341435985952545E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21">
+        <v>0.57412009696045196</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>0.57773605097509795</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="11">
+        <f>SUM(G17:G20)</f>
+        <v>290.80919611991754</v>
+      </c>
+      <c r="H21" s="11">
+        <f>SUM(H17:H20)</f>
+        <v>263.25769755627499</v>
+      </c>
+      <c r="I21" s="13">
+        <f t="shared" si="1"/>
+        <v>-9.4740809201513287E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22">
+        <v>0.71368713748379498</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <v>0.72638774745941903</v>
+      </c>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23">
+        <v>27.304571051796898</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23">
+        <v>45.806088617262702</v>
+      </c>
+      <c r="E23" s="6"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24">
+        <v>318.11376717171498</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24">
+        <v>309.06378617353801</v>
+      </c>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="E25" s="6"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="E26" s="6"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="E27" s="6"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="E29" s="6"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="E30" s="6"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="E31" s="6"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="5:5">
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="5:5">
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="5:5">
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="5:5">
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="5:5">
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="5:5">
+      <c r="E43" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+      <selection activeCell="D17" sqref="A12:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="3" width="10.125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="B1" t="s">
@@ -6895,7 +6725,34 @@
     <row r="11" spans="1:15">
       <c r="D11" s="1"/>
     </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
     <row r="13" spans="1:15">
+      <c r="A13" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10.2773689376482</v>
+      </c>
+      <c r="C13" s="7">
+        <v>6.2822829115338701</v>
+      </c>
+      <c r="D13" s="12">
+        <f>C13/B13</f>
+        <v>0.61127346402059424</v>
+      </c>
       <c r="H13" t="s">
         <v>12</v>
       </c>
@@ -6909,7 +6766,35 @@
         <v>11</v>
       </c>
     </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="7">
+        <v>1.6786557270081099</v>
+      </c>
+      <c r="C14" s="7">
+        <v>1.0474309294178099</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" ref="D13:D16" si="1">C14/B14</f>
+        <v>0.6239700687672628</v>
+      </c>
+    </row>
     <row r="15" spans="1:15">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="7">
+        <v>399.07159617236698</v>
+      </c>
+      <c r="C15" s="7">
+        <v>245.89278461090899</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="1"/>
+        <v>0.61616207961015346</v>
+      </c>
       <c r="I15">
         <v>9.8461892259614903</v>
       </c>
@@ -6930,6 +6815,19 @@
       </c>
     </row>
     <row r="16" spans="1:15">
+      <c r="A16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="7">
+        <v>4.3045918833761094</v>
+      </c>
+      <c r="C16" s="7">
+        <v>4.4171913154808875</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="1"/>
+        <v>1.0261579808621639</v>
+      </c>
       <c r="I16">
         <v>1.61700734253365</v>
       </c>
@@ -6949,7 +6847,23 @@
         <v>38.359602376872999</v>
       </c>
     </row>
-    <row r="17" spans="9:15">
+    <row r="17" spans="1:15">
+      <c r="A17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8">
+        <f>SUM(B13:B16)</f>
+        <v>415.33221272039941</v>
+      </c>
+      <c r="C17" s="8">
+        <f>SUM(C13:C16)</f>
+        <v>257.63968976734157</v>
+      </c>
+      <c r="D17" s="13">
+        <f>C17/B17</f>
+        <v>0.62032195403245538</v>
+      </c>
+      <c r="E17" s="2"/>
       <c r="I17">
         <v>383.65287528670302</v>
       </c>
@@ -6969,7 +6883,7 @@
         <v>39.0997185688869</v>
       </c>
     </row>
-    <row r="18" spans="9:15">
+    <row r="18" spans="1:15">
       <c r="I18">
         <v>0.15275599185576499</v>
       </c>
@@ -6989,7 +6903,7 @@
         <v>42.929812318502499</v>
       </c>
     </row>
-    <row r="19" spans="9:15">
+    <row r="19" spans="1:15">
       <c r="I19">
         <v>4.0992379503754703</v>
       </c>
@@ -7009,7 +6923,7 @@
         <v>-3.9784216383072599</v>
       </c>
     </row>
-    <row r="20" spans="9:15">
+    <row r="20" spans="1:15">
       <c r="I20">
         <v>16.098590877214299</v>
       </c>
@@ -7029,7 +6943,7 @@
         <v>-14.790960084062799</v>
       </c>
     </row>
-    <row r="21" spans="9:15">
+    <row r="21" spans="1:15">
       <c r="I21">
         <v>415.46665667464401</v>
       </c>
@@ -7157,5 +7071,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>